<commit_message>
update sample and api list
</commit_message>
<xml_diff>
--- a/api-instruction.xlsx
+++ b/api-instruction.xlsx
@@ -1288,6 +1288,7 @@
         <color rgb="FF00A65D"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3、AppUtils接口
 </t>
@@ -1297,6 +1298,7 @@
         <sz val="11"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">startApp(String pkg, String clazz, String type, String title, String uri, String info)</t>
     </r>
@@ -1318,127 +1320,16 @@
     <t xml:space="preserve">浏览器</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">、命令行
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Adb shell am start -a android.intent.action.VIEW -d </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://www.baidu.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> org.chromium.chrome
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Java</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">代码
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Intent intent = new Intent("android.intent.action.VIEW");
+    <t xml:space="preserve">1、命令行
+Adb shell am start -a android.intent.action.VIEW -d http://www.baidu.com org.chromium.chrome
+2、Java代码
+Intent intent = new Intent("android.intent.action.VIEW");
 intent.setData(Uri.parse(url));
 intent.setPackage("org.chromium.chrome");
 intent.setFlags(Intent.FLAG_ACTIVITY_NEW_TASK);
 startActivity(intent);
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">3、AppUtils接口
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Noto Sans Mono CJK JP Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">openBrowser(String url)</t>
-    </r>
+3、AppUtils接口
+openBrowser(String url)</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1542,28 +1433,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF00A65D"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans Mono CJK JP Regular"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1716,7 +1589,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1800,11 +1673,9 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="C74" activeCellId="0" sqref="C74"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3919,7 +3790,7 @@
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://www.baidu.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="1、命令行&#10;Adb shell am start -a android.intent.action.VIEW -d http://www.baidu.com org.chromium.chrome&#10;2、Java代码&#10;Intent intent = new Intent(&quot;android.intent.action.VIEW&quot;);&#10;intent.setData(Uri.parse(url));&#10;intent.setPackage(&quot;org.chromium.chrome&quot;);&#10;intent.setFlags(Intent.FLAG_ACTIVITY_NEW_TASK);&#10;startActivity(intent);&#10;3、AppUtils接口&#10;openBrowser(String url)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>